<commit_message>
Measurement organisation and fit
</commit_message>
<xml_diff>
--- a/WO3189/1024_1258_wo3189_r13 RT1/H2 drop fit/1024_1258_wo3189_r13_resistance_fit_coef.xlsx
+++ b/WO3189/1024_1258_wo3189_r13 RT1/H2 drop fit/1024_1258_wo3189_r13_resistance_fit_coef.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rijk\Documents\MEP\MEP_control_software\1024_1258_wo3189_r13 RT1\data\H2 drop fit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rijk\Documents\MEP\MEP_control_software\Measurements\1024_1258_wo3189_r13 RT1\H2 drop fit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C20A164-9EF3-412B-8E1E-B849F4FD1D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05680102-2F88-42F5-95BC-F84EEE0807FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -506,9 +508,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -867,7 +870,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +898,7 @@
         <f>B2*A2</f>
         <v>7.6024230772141514E-3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <f>C2^-1</f>
         <v>131.53700995636279</v>
       </c>

</xml_diff>